<commit_message>
Updated to last graph-theory version
The main change is the usage of the new version of graph-theory, although there are some changes in preliminaries.v, dom.v, wirred.v and check.v to adjust them to the new version. In addition, coloring.v has some (yet not matured) definitions of graoh colorings.
</commit_message>
<xml_diff>
--- a/solver/instances/BuenosAires.xlsx
+++ b/solver/instances/BuenosAires.xlsx
@@ -306,12 +306,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -330,7 +336,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
@@ -352,6 +358,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -650,7 +670,7 @@
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1404,8 +1424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1485,37 +1505,39 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="3">
+      <c r="A5" s="10">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="13">
         <v>138942</v>
       </c>
-      <c r="F5" s="2">
+      <c r="E5" s="14"/>
+      <c r="F5" s="9">
         <f t="shared" si="0"/>
         <v>138.94200000000001</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="3">
+      <c r="A6" s="10">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="13">
         <v>89360</v>
       </c>
-      <c r="F6" s="2">
+      <c r="E6" s="14"/>
+      <c r="F6" s="9">
         <f t="shared" si="0"/>
         <v>89.36</v>
       </c>
@@ -1539,19 +1561,20 @@
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="3">
+      <c r="A8" s="10">
         <v>6</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="13">
         <v>39473</v>
       </c>
-      <c r="F8" s="2">
+      <c r="E8" s="14"/>
+      <c r="F8" s="9">
         <f t="shared" si="0"/>
         <v>39.472999999999999</v>
       </c>
@@ -1593,19 +1616,20 @@
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="3">
+      <c r="A11" s="10">
         <v>9</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="13">
         <v>252312</v>
       </c>
-      <c r="F11" s="2">
+      <c r="E11" s="14"/>
+      <c r="F11" s="9">
         <f t="shared" si="0"/>
         <v>252.31200000000001</v>
       </c>
@@ -1629,19 +1653,20 @@
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="3">
+      <c r="A13" s="10">
         <v>11</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="13">
         <v>71013</v>
       </c>
-      <c r="F13" s="2">
+      <c r="E13" s="14"/>
+      <c r="F13" s="9">
         <f t="shared" si="0"/>
         <v>71.013000000000005</v>
       </c>
@@ -1719,19 +1744,20 @@
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="3">
+      <c r="A18" s="10">
         <v>16</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="13">
         <v>188780</v>
       </c>
-      <c r="F18" s="2">
+      <c r="E18" s="14"/>
+      <c r="F18" s="9">
         <f t="shared" si="0"/>
         <v>188.78</v>
       </c>
@@ -1755,19 +1781,20 @@
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="3">
+      <c r="A20" s="10">
         <v>18</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="13">
         <v>14278</v>
       </c>
-      <c r="F20" s="2">
+      <c r="E20" s="14"/>
+      <c r="F20" s="9">
         <f t="shared" si="0"/>
         <v>14.278</v>
       </c>
@@ -1827,19 +1854,20 @@
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="3">
+      <c r="A24" s="10">
         <v>22</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="13">
         <v>183396</v>
       </c>
-      <c r="F24" s="2">
+      <c r="E24" s="14"/>
+      <c r="F24" s="9">
         <f t="shared" si="0"/>
         <v>183.39599999999999</v>
       </c>
@@ -1863,19 +1891,20 @@
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="3">
+      <c r="A26" s="10">
         <v>24</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="13">
         <v>152198</v>
       </c>
-      <c r="F26" s="2">
+      <c r="E26" s="14"/>
+      <c r="F26" s="9">
         <f t="shared" si="0"/>
         <v>152.19800000000001</v>
       </c>
@@ -1989,19 +2018,20 @@
       </c>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="3">
+      <c r="A33" s="10">
         <v>31</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D33" s="5">
+      <c r="D33" s="13">
         <v>150484</v>
       </c>
-      <c r="F33" s="2">
+      <c r="E33" s="14"/>
+      <c r="F33" s="9">
         <f t="shared" si="0"/>
         <v>150.48400000000001</v>
       </c>
@@ -2133,37 +2163,39 @@
       </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="3">
+      <c r="A41" s="10">
         <v>39</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D41" s="5">
+      <c r="D41" s="13">
         <v>64932</v>
       </c>
-      <c r="F41" s="2">
+      <c r="E41" s="14"/>
+      <c r="F41" s="9">
         <f t="shared" si="0"/>
         <v>64.932000000000002</v>
       </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="3">
+      <c r="A42" s="10">
         <v>40</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D42" s="5">
+      <c r="D42" s="13">
         <v>54191</v>
       </c>
-      <c r="F42" s="2">
+      <c r="E42" s="14"/>
+      <c r="F42" s="9">
         <f t="shared" si="0"/>
         <v>54.191000000000003</v>
       </c>
@@ -2205,55 +2237,58 @@
       </c>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="3">
+      <c r="A45" s="10">
         <v>43</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C45" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D45" s="5">
+      <c r="D45" s="13">
         <v>77474</v>
       </c>
-      <c r="F45" s="2">
+      <c r="E45" s="14"/>
+      <c r="F45" s="9">
         <f t="shared" si="0"/>
         <v>77.474000000000004</v>
       </c>
     </row>
     <row r="46" spans="1:6">
-      <c r="A46" s="3">
+      <c r="A46" s="10">
         <v>44</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D46" s="5">
+      <c r="D46" s="13">
         <v>46494</v>
       </c>
-      <c r="F46" s="2">
+      <c r="E46" s="14"/>
+      <c r="F46" s="9">
         <f t="shared" si="0"/>
         <v>46.494</v>
       </c>
     </row>
     <row r="47" spans="1:6">
-      <c r="A47" s="3">
+      <c r="A47" s="10">
         <v>45</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C47" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="D47" s="5">
+      <c r="D47" s="13">
         <v>114253</v>
       </c>
-      <c r="F47" s="2">
+      <c r="E47" s="14"/>
+      <c r="F47" s="9">
         <f t="shared" si="0"/>
         <v>114.253</v>
       </c>

</xml_diff>